<commit_message>
visualization moved to external notebook
</commit_message>
<xml_diff>
--- a/notebooks/output/values.xlsx
+++ b/notebooks/output/values.xlsx
@@ -474,19 +474,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6455000042915344</v>
+        <v>0.6290000081062317</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6460925833748133</v>
+        <v>0.627177700348432</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5390741662518665</v>
+        <v>0.5326032852165257</v>
       </c>
       <c r="F2" t="n">
-        <v>0.646590343454455</v>
+        <v>0.6291687406669985</v>
       </c>
       <c r="G2" t="n">
-        <v>0.532105525136884</v>
+        <v>0.5286212045793928</v>
       </c>
     </row>
     <row r="3">
@@ -497,19 +497,19 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6389999985694885</v>
+        <v>0.6445000171661377</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6366351418616227</v>
+        <v>0.6450970632155301</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5306122448979592</v>
+        <v>0.5340965654554505</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6386261821801892</v>
+        <v>0.6445993031358885</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5370831259333001</v>
+        <v>0.5425584868093579</v>
       </c>
     </row>
     <row r="4">
@@ -520,19 +520,19 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6324999928474426</v>
+        <v>0.6380000114440918</v>
       </c>
       <c r="D4" t="n">
-        <v>0.633648581383773</v>
+        <v>0.6386261821801892</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5062220009955202</v>
+        <v>0.5460428073668492</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6316575410652066</v>
+        <v>0.640119462419114</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5281234444997511</v>
+        <v>0.5375808860129417</v>
       </c>
     </row>
     <row r="5">
@@ -543,19 +543,19 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6330000162124634</v>
+        <v>0.6345000267028809</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6341463414634146</v>
+        <v>0.6331508213041314</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5470383275261324</v>
+        <v>0.5316077650572424</v>
       </c>
       <c r="F5" t="n">
-        <v>0.633648581383773</v>
+        <v>0.6346441015430563</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5251368840219014</v>
+        <v>0.5151816824290691</v>
       </c>
     </row>
     <row r="6">
@@ -566,19 +566,19 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6455000042915344</v>
+        <v>0.6355000138282776</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6445993031358885</v>
+        <v>0.6376306620209059</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5291189646590343</v>
+        <v>0.5306122448979592</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6460925833748133</v>
+        <v>0.6346441015430563</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5271279243404678</v>
+        <v>0.5226480836236934</v>
       </c>
     </row>
     <row r="7">
@@ -589,19 +589,19 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6439999938011169</v>
+        <v>0.6430000066757202</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6445993031358885</v>
+        <v>0.6441015430562469</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5335988053758088</v>
+        <v>0.5281234444997511</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6411149825783972</v>
+        <v>0.6436037829766053</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5375808860129417</v>
+        <v>0.5211548033847685</v>
       </c>
     </row>
     <row r="8">
@@ -612,19 +612,19 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6430000066757202</v>
+        <v>0.6395000219345093</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6441015430562469</v>
+        <v>0.6406172224987556</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5380786460925834</v>
+        <v>0.5530114484818317</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6441015430562469</v>
+        <v>0.6411149825783972</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5440517670482827</v>
+        <v>0.560477849676456</v>
       </c>
     </row>
     <row r="9">
@@ -635,19 +635,19 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6345000267028809</v>
+        <v>0.6430000066757202</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6331508213041314</v>
+        <v>0.6455948232951717</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5052264808362369</v>
+        <v>0.5316077650572424</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6366351418616227</v>
+        <v>0.6441015430562469</v>
       </c>
       <c r="G9" t="n">
-        <v>0.5266301642608263</v>
+        <v>0.5435540069686411</v>
       </c>
     </row>
     <row r="10">
@@ -658,19 +658,19 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6399999856948853</v>
+        <v>0.640999972820282</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6391239422598307</v>
+        <v>0.6411149825783972</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5301144848183176</v>
+        <v>0.5151816824290691</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6396217023394724</v>
+        <v>0.6416127426580388</v>
       </c>
       <c r="G10" t="n">
-        <v>0.5350920856147336</v>
+        <v>0.5360876057740169</v>
       </c>
     </row>
     <row r="11">
@@ -681,19 +681,19 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6370000243186951</v>
+        <v>0.6499999761581421</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6391239422598307</v>
+        <v>0.6485813837730214</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5425584868093579</v>
+        <v>0.5231458437033349</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6386261821801892</v>
+        <v>0.6495769039323046</v>
       </c>
       <c r="G11" t="n">
-        <v>0.5340965654554505</v>
+        <v>0.547536087605774</v>
       </c>
     </row>
     <row r="12">
@@ -704,19 +704,19 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6445000171661377</v>
+        <v>0.6359999775886536</v>
       </c>
       <c r="D12" t="n">
-        <v>0.6436037829766053</v>
+        <v>0.6376306620209059</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5435540069686411</v>
+        <v>0.5266301642608263</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6411149825783972</v>
+        <v>0.6366351418616227</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5306122448979592</v>
+        <v>0.5186660029865605</v>
       </c>
     </row>
     <row r="13">
@@ -727,19 +727,19 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6365000009536743</v>
+        <v>0.6420000195503235</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6386261821801892</v>
+        <v>0.6416127426580388</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5146839223494276</v>
+        <v>0.5072175211548033</v>
       </c>
       <c r="F13" t="n">
-        <v>0.6406172224987556</v>
+        <v>0.6421105027376804</v>
       </c>
       <c r="G13" t="n">
-        <v>0.532105525136884</v>
+        <v>0.538576406172225</v>
       </c>
     </row>
     <row r="14">
@@ -750,19 +750,19 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6365000009536743</v>
+        <v>0.6414999961853027</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6376306620209059</v>
+        <v>0.6411149825783972</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5360876057740169</v>
+        <v>0.5311100049776007</v>
       </c>
       <c r="F14" t="n">
-        <v>0.6366351418616227</v>
+        <v>0.6411149825783972</v>
       </c>
       <c r="G14" t="n">
-        <v>0.5375808860129417</v>
+        <v>0.5156794425087108</v>
       </c>
     </row>
     <row r="15">
@@ -773,19 +773,19 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6474999785423279</v>
+        <v>0.6579999923706055</v>
       </c>
       <c r="D15" t="n">
-        <v>0.6460925833748133</v>
+        <v>0.658038825286212</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5151816824290691</v>
+        <v>0.5176704828272772</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6485813837730214</v>
+        <v>0.6570433051269288</v>
       </c>
       <c r="G15" t="n">
-        <v>0.5221503235440518</v>
+        <v>0.5440517670482827</v>
       </c>
     </row>
     <row r="16">
@@ -796,19 +796,19 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>0.6345000267028809</v>
+        <v>0.6365000009536743</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6346441015430563</v>
+        <v>0.6366351418616227</v>
       </c>
       <c r="E16" t="n">
-        <v>0.5470383275261324</v>
+        <v>0.5629666500746641</v>
       </c>
       <c r="F16" t="n">
-        <v>0.6326530612244898</v>
+        <v>0.6361373817819811</v>
       </c>
       <c r="G16" t="n">
-        <v>0.5440517670482827</v>
+        <v>0.5559980089596814</v>
       </c>
     </row>
     <row r="17">
@@ -819,19 +819,19 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>0.6284999847412109</v>
+        <v>0.6334999799728394</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6296665007466401</v>
+        <v>0.6326530612244898</v>
       </c>
       <c r="E17" t="n">
-        <v>0.5171727227476356</v>
+        <v>0.5246391239422599</v>
       </c>
       <c r="F17" t="n">
-        <v>0.6291687406669985</v>
+        <v>0.6331508213041314</v>
       </c>
       <c r="G17" t="n">
-        <v>0.5111996017919362</v>
+        <v>0.5311100049776007</v>
       </c>
     </row>
     <row r="18">
@@ -842,19 +842,19 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>0.637499988079071</v>
+        <v>0.6359999775886536</v>
       </c>
       <c r="D18" t="n">
         <v>0.6381284221005475</v>
       </c>
       <c r="E18" t="n">
-        <v>0.520657043305127</v>
+        <v>0.5316077650572424</v>
       </c>
       <c r="F18" t="n">
         <v>0.6381284221005475</v>
       </c>
       <c r="G18" t="n">
-        <v>0.5176704828272772</v>
+        <v>0.5246391239422599</v>
       </c>
     </row>
     <row r="19">
@@ -865,19 +865,19 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6320000290870667</v>
+        <v>0.6414999961853027</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6331508213041314</v>
+        <v>0.6406172224987556</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5301144848183176</v>
+        <v>0.538576406172225</v>
       </c>
       <c r="F19" t="n">
-        <v>0.6331508213041314</v>
+        <v>0.6416127426580388</v>
       </c>
       <c r="G19" t="n">
-        <v>0.541065206570433</v>
+        <v>0.5156794425087108</v>
       </c>
     </row>
     <row r="20">
@@ -888,19 +888,19 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6470000147819519</v>
+        <v>0.6424999833106995</v>
       </c>
       <c r="D20" t="n">
-        <v>0.6445993031358885</v>
+        <v>0.6426082628173221</v>
       </c>
       <c r="E20" t="n">
-        <v>0.5360876057740169</v>
+        <v>0.5261324041811847</v>
       </c>
       <c r="F20" t="n">
-        <v>0.646590343454455</v>
+        <v>0.6426082628173221</v>
       </c>
       <c r="G20" t="n">
-        <v>0.5296167247386759</v>
+        <v>0.5271279243404678</v>
       </c>
     </row>
     <row r="21">
@@ -911,19 +911,19 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6430000066757202</v>
+        <v>0.6420000195503235</v>
       </c>
       <c r="D21" t="n">
+        <v>0.6450970632155301</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.5515181682429069</v>
+      </c>
+      <c r="F21" t="n">
         <v>0.6436037829766053</v>
       </c>
-      <c r="E21" t="n">
-        <v>0.5350920856147336</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.6426082628173221</v>
-      </c>
       <c r="G21" t="n">
-        <v>0.5415629666500746</v>
+        <v>0.5271279243404678</v>
       </c>
     </row>
     <row r="22">
@@ -934,19 +934,19 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6330000162124634</v>
+        <v>0.6324999928474426</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6311597809855649</v>
+        <v>0.6306620209059234</v>
       </c>
       <c r="E22" t="n">
-        <v>0.5316077650572424</v>
+        <v>0.5286212045793928</v>
       </c>
       <c r="F22" t="n">
-        <v>0.6316575410652066</v>
+        <v>0.6321553011448482</v>
       </c>
       <c r="G22" t="n">
-        <v>0.5156794425087108</v>
+        <v>0.5311100049776007</v>
       </c>
     </row>
     <row r="23">
@@ -957,19 +957,19 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0.6265000104904175</v>
+        <v>0.6489999890327454</v>
       </c>
       <c r="D23" t="n">
-        <v>0.627177700348432</v>
+        <v>0.6540567446490791</v>
       </c>
       <c r="E23" t="n">
-        <v>0.525634644101543</v>
+        <v>0.5186660029865605</v>
       </c>
       <c r="F23" t="n">
-        <v>0.6251866600298656</v>
+        <v>0.6470881035340965</v>
       </c>
       <c r="G23" t="n">
-        <v>0.5216525634644101</v>
+        <v>0.5136884021901443</v>
       </c>
     </row>
     <row r="24">
@@ -980,19 +980,19 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0.6384999752044678</v>
+        <v>0.6330000162124634</v>
       </c>
       <c r="D24" t="n">
-        <v>0.6391239422598307</v>
+        <v>0.6316575410652066</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5291189646590343</v>
+        <v>0.5241413638626182</v>
       </c>
       <c r="F24" t="n">
-        <v>0.640119462419114</v>
+        <v>0.6326530612244898</v>
       </c>
       <c r="G24" t="n">
-        <v>0.5186660029865605</v>
+        <v>0.5445495271279244</v>
       </c>
     </row>
     <row r="25">
@@ -1003,19 +1003,19 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0.6234999895095825</v>
+        <v>0.6399999856948853</v>
       </c>
       <c r="D25" t="n">
-        <v>0.6241911398705824</v>
+        <v>0.6346441015430563</v>
       </c>
       <c r="E25" t="n">
-        <v>0.5296167247386759</v>
+        <v>0.5360876057740169</v>
       </c>
       <c r="F25" t="n">
-        <v>0.6217023394723743</v>
+        <v>0.6386261821801892</v>
       </c>
       <c r="G25" t="n">
-        <v>0.538576406172225</v>
+        <v>0.5286212045793928</v>
       </c>
     </row>
     <row r="26">
@@ -1026,19 +1026,19 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.6520000100135803</v>
+        <v>0.6449999809265137</v>
       </c>
       <c r="D26" t="n">
-        <v>0.6525634644101543</v>
+        <v>0.6455948232951717</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5395719263315082</v>
+        <v>0.5415629666500746</v>
       </c>
       <c r="F26" t="n">
-        <v>0.649079143852663</v>
+        <v>0.6445993031358885</v>
       </c>
       <c r="G26" t="n">
-        <v>0.541065206570433</v>
+        <v>0.5146839223494276</v>
       </c>
     </row>
     <row r="27">
@@ -1049,19 +1049,19 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>0.6359999775886536</v>
+        <v>0.6365000009536743</v>
       </c>
       <c r="D27" t="n">
-        <v>0.633648581383773</v>
+        <v>0.6356396217023395</v>
       </c>
       <c r="E27" t="n">
-        <v>0.532105525136884</v>
+        <v>0.525634644101543</v>
       </c>
       <c r="F27" t="n">
         <v>0.6356396217023395</v>
       </c>
       <c r="G27" t="n">
-        <v>0.5276256844201095</v>
+        <v>0.5296167247386759</v>
       </c>
     </row>
     <row r="28">
@@ -1072,19 +1072,19 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>0.6290000081062317</v>
+        <v>0.6470000147819519</v>
       </c>
       <c r="D28" t="n">
-        <v>0.6256844201095072</v>
+        <v>0.6431060228969636</v>
       </c>
       <c r="E28" t="n">
-        <v>0.5236436037829766</v>
+        <v>0.5181682429069189</v>
       </c>
       <c r="F28" t="n">
-        <v>0.6296665007466401</v>
+        <v>0.6445993031358885</v>
       </c>
       <c r="G28" t="n">
-        <v>0.5276256844201095</v>
+        <v>0.5171727227476356</v>
       </c>
     </row>
     <row r="29">
@@ -1095,19 +1095,19 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>0.6445000171661377</v>
+        <v>0.6420000195503235</v>
       </c>
       <c r="D29" t="n">
-        <v>0.6450970632155301</v>
+        <v>0.6391239422598307</v>
       </c>
       <c r="E29" t="n">
-        <v>0.5440517670482827</v>
+        <v>0.5375808860129417</v>
       </c>
       <c r="F29" t="n">
-        <v>0.6455948232951717</v>
+        <v>0.6396217023394724</v>
       </c>
       <c r="G29" t="n">
-        <v>0.5311100049776007</v>
+        <v>0.5331010452961672</v>
       </c>
     </row>
     <row r="30">
@@ -1118,19 +1118,19 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>0.6420000195503235</v>
+        <v>0.628000020980835</v>
       </c>
       <c r="D30" t="n">
-        <v>0.6416127426580388</v>
+        <v>0.6286709805873569</v>
       </c>
       <c r="E30" t="n">
-        <v>0.5340965654554505</v>
+        <v>0.5201592832254853</v>
       </c>
       <c r="F30" t="n">
-        <v>0.6406172224987556</v>
+        <v>0.6311597809855649</v>
       </c>
       <c r="G30" t="n">
-        <v>0.5435540069686411</v>
+        <v>0.4947735191637631</v>
       </c>
     </row>
     <row r="31">
@@ -1141,19 +1141,19 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>0.6430000066757202</v>
+        <v>0.6395000219345093</v>
       </c>
       <c r="D31" t="n">
-        <v>0.6431060228969636</v>
+        <v>0.6436037829766053</v>
       </c>
       <c r="E31" t="n">
-        <v>0.5445495271279244</v>
+        <v>0.5042309606769537</v>
       </c>
       <c r="F31" t="n">
-        <v>0.6436037829766053</v>
+        <v>0.640119462419114</v>
       </c>
       <c r="G31" t="n">
-        <v>0.5510204081632653</v>
+        <v>0.5126928820308612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>